<commit_message>
rename files, add spatial DG features to Player.java and add SpatialEvoDG2.java
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -48,10 +48,10 @@
     <t>N: 100</t>
   </si>
   <si>
-    <t>Gens: 10000</t>
+    <t>Gens: 1000000</t>
   </si>
   <si>
-    <t>Program: SpatialEvoDG1</t>
+    <t>Program: SpatialEvoDG2</t>
   </si>
 </sst>
 </file>
@@ -87,8 +87,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,210 +394,211 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="2" customWidth="1"/>
-    <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="2" customWidth="1"/>
-    <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="2" customWidth="1"/>
-    <col min="14" max="14" width="12" customWidth="1"/>
-    <col min="15" max="15" width="2" customWidth="1"/>
-    <col min="16" max="16" width="12" customWidth="1"/>
-    <col min="17" max="17" width="2" customWidth="1"/>
-    <col min="18" max="18" width="12" customWidth="1"/>
-    <col min="19" max="19" width="2" customWidth="1"/>
-    <col min="20" max="20" width="12" customWidth="1"/>
-    <col min="21" max="21" width="3" customWidth="1"/>
-    <col min="22" max="22" width="12" customWidth="1"/>
-    <col min="23" max="23" width="3" customWidth="1"/>
-    <col min="24" max="24" width="12" customWidth="1"/>
-    <col min="25" max="25" width="3" customWidth="1"/>
-    <col min="26" max="26" width="11" customWidth="1"/>
-    <col min="27" max="27" width="3" customWidth="1"/>
-    <col min="28" max="28" width="12" customWidth="1"/>
-    <col min="29" max="29" width="3" customWidth="1"/>
-    <col min="30" max="30" width="10" customWidth="1"/>
-    <col min="31" max="31" width="3" customWidth="1"/>
-    <col min="32" max="32" width="12" customWidth="1"/>
-    <col min="33" max="33" width="3" customWidth="1"/>
-    <col min="34" max="34" width="12" customWidth="1"/>
-    <col min="35" max="35" width="3" customWidth="1"/>
-    <col min="36" max="36" width="12" customWidth="1"/>
-    <col min="37" max="37" width="3" customWidth="1"/>
-    <col min="38" max="38" width="12" customWidth="1"/>
-    <col min="39" max="39" width="3" customWidth="1"/>
-    <col min="40" max="40" width="12" customWidth="1"/>
-    <col min="41" max="41" width="3" customWidth="1"/>
-    <col min="42" max="42" width="12" customWidth="1"/>
-    <col min="43" max="43" width="3" customWidth="1"/>
-    <col min="44" max="44" width="11" customWidth="1"/>
-    <col min="45" max="45" width="3" customWidth="1"/>
-    <col min="46" max="46" width="12" customWidth="1"/>
-    <col min="47" max="47" width="3" customWidth="1"/>
-    <col min="48" max="48" width="12" customWidth="1"/>
-    <col min="49" max="49" width="3" customWidth="1"/>
-    <col min="50" max="50" width="12" customWidth="1"/>
-    <col min="51" max="51" width="3" customWidth="1"/>
-    <col min="52" max="52" width="12" customWidth="1"/>
-    <col min="53" max="53" width="3" customWidth="1"/>
-    <col min="54" max="54" width="12" customWidth="1"/>
-    <col min="55" max="55" width="3" customWidth="1"/>
-    <col min="56" max="56" width="12" customWidth="1"/>
-    <col min="57" max="57" width="3" customWidth="1"/>
-    <col min="58" max="58" width="12" customWidth="1"/>
-    <col min="59" max="59" width="3" customWidth="1"/>
-    <col min="60" max="60" width="12" customWidth="1"/>
-    <col min="61" max="61" width="3" customWidth="1"/>
-    <col min="62" max="62" width="12" customWidth="1"/>
-    <col min="63" max="63" width="3" customWidth="1"/>
-    <col min="64" max="64" width="12" customWidth="1"/>
-    <col min="65" max="65" width="3" customWidth="1"/>
-    <col min="66" max="66" width="12" customWidth="1"/>
-    <col min="67" max="67" width="3" customWidth="1"/>
-    <col min="68" max="68" width="12" customWidth="1"/>
-    <col min="69" max="69" width="3" customWidth="1"/>
-    <col min="70" max="70" width="12" customWidth="1"/>
-    <col min="71" max="71" width="3" customWidth="1"/>
-    <col min="72" max="72" width="12" customWidth="1"/>
-    <col min="73" max="73" width="3" customWidth="1"/>
-    <col min="74" max="74" width="12" customWidth="1"/>
-    <col min="75" max="75" width="3" customWidth="1"/>
-    <col min="76" max="76" width="12" customWidth="1"/>
-    <col min="77" max="77" width="3" customWidth="1"/>
-    <col min="78" max="78" width="12" customWidth="1"/>
-    <col min="79" max="79" width="3" customWidth="1"/>
-    <col min="80" max="80" width="12" customWidth="1"/>
-    <col min="81" max="81" width="3" customWidth="1"/>
-    <col min="82" max="82" width="12" customWidth="1"/>
-    <col min="83" max="83" width="3" customWidth="1"/>
-    <col min="84" max="84" width="11" customWidth="1"/>
-    <col min="85" max="85" width="3" customWidth="1"/>
-    <col min="86" max="86" width="12" customWidth="1"/>
-    <col min="87" max="87" width="3" customWidth="1"/>
-    <col min="88" max="88" width="12" customWidth="1"/>
-    <col min="89" max="89" width="3" customWidth="1"/>
-    <col min="90" max="90" width="11" customWidth="1"/>
-    <col min="91" max="91" width="3" customWidth="1"/>
-    <col min="92" max="92" width="12" customWidth="1"/>
-    <col min="93" max="93" width="3" customWidth="1"/>
-    <col min="94" max="94" width="12" customWidth="1"/>
-    <col min="95" max="95" width="3" customWidth="1"/>
-    <col min="96" max="96" width="12" customWidth="1"/>
-    <col min="97" max="97" width="3" customWidth="1"/>
-    <col min="98" max="98" width="12" customWidth="1"/>
-    <col min="99" max="99" width="3" customWidth="1"/>
-    <col min="100" max="100" width="12" customWidth="1"/>
-    <col min="101" max="101" width="3" customWidth="1"/>
-    <col min="102" max="102" width="12" customWidth="1"/>
-    <col min="103" max="103" width="3" customWidth="1"/>
-    <col min="104" max="104" width="12" customWidth="1"/>
-    <col min="105" max="105" width="3" customWidth="1"/>
-    <col min="106" max="106" width="12" customWidth="1"/>
-    <col min="107" max="107" width="3" customWidth="1"/>
-    <col min="108" max="108" width="12" customWidth="1"/>
-    <col min="109" max="109" width="3" customWidth="1"/>
-    <col min="110" max="110" width="12" customWidth="1"/>
-    <col min="111" max="111" width="3" customWidth="1"/>
-    <col min="112" max="112" width="12" customWidth="1"/>
-    <col min="113" max="113" width="3" customWidth="1"/>
-    <col min="114" max="114" width="12" customWidth="1"/>
-    <col min="115" max="115" width="3" customWidth="1"/>
-    <col min="116" max="116" width="12" customWidth="1"/>
-    <col min="117" max="117" width="3" customWidth="1"/>
-    <col min="118" max="118" width="12" customWidth="1"/>
-    <col min="119" max="119" width="3" customWidth="1"/>
-    <col min="120" max="120" width="12" customWidth="1"/>
-    <col min="121" max="121" width="3" customWidth="1"/>
-    <col min="122" max="122" width="12" customWidth="1"/>
-    <col min="123" max="123" width="3" customWidth="1"/>
-    <col min="124" max="124" width="12" customWidth="1"/>
-    <col min="125" max="125" width="3" customWidth="1"/>
-    <col min="126" max="126" width="12" customWidth="1"/>
-    <col min="127" max="127" width="3" customWidth="1"/>
-    <col min="128" max="128" width="12" customWidth="1"/>
-    <col min="129" max="129" width="3" customWidth="1"/>
-    <col min="130" max="130" width="10" customWidth="1"/>
-    <col min="131" max="131" width="3" customWidth="1"/>
-    <col min="132" max="132" width="12" customWidth="1"/>
-    <col min="133" max="133" width="3" customWidth="1"/>
-    <col min="134" max="134" width="12" customWidth="1"/>
-    <col min="135" max="135" width="3" customWidth="1"/>
-    <col min="136" max="136" width="12" customWidth="1"/>
-    <col min="137" max="137" width="3" customWidth="1"/>
-    <col min="138" max="138" width="12" customWidth="1"/>
-    <col min="139" max="139" width="3" customWidth="1"/>
-    <col min="140" max="140" width="12" customWidth="1"/>
-    <col min="141" max="141" width="3" customWidth="1"/>
-    <col min="142" max="142" width="12" customWidth="1"/>
-    <col min="143" max="143" width="3" customWidth="1"/>
-    <col min="144" max="144" width="12" customWidth="1"/>
-    <col min="145" max="145" width="3" customWidth="1"/>
-    <col min="146" max="146" width="12" customWidth="1"/>
-    <col min="147" max="147" width="3" customWidth="1"/>
-    <col min="148" max="148" width="12" customWidth="1"/>
-    <col min="149" max="149" width="3" customWidth="1"/>
-    <col min="150" max="150" width="12" customWidth="1"/>
-    <col min="151" max="151" width="3" customWidth="1"/>
-    <col min="152" max="152" width="12" customWidth="1"/>
-    <col min="153" max="153" width="3" customWidth="1"/>
-    <col min="154" max="154" width="12" customWidth="1"/>
-    <col min="155" max="155" width="3" customWidth="1"/>
-    <col min="156" max="156" width="12" customWidth="1"/>
-    <col min="157" max="157" width="3" customWidth="1"/>
-    <col min="158" max="158" width="12" customWidth="1"/>
-    <col min="159" max="159" width="3" customWidth="1"/>
-    <col min="160" max="160" width="12" customWidth="1"/>
-    <col min="161" max="161" width="3" customWidth="1"/>
-    <col min="162" max="162" width="12" customWidth="1"/>
-    <col min="163" max="163" width="3" customWidth="1"/>
-    <col min="164" max="164" width="12" customWidth="1"/>
-    <col min="165" max="165" width="3" customWidth="1"/>
-    <col min="166" max="166" width="12" customWidth="1"/>
-    <col min="167" max="167" width="3" customWidth="1"/>
-    <col min="168" max="168" width="12" customWidth="1"/>
-    <col min="169" max="169" width="3" customWidth="1"/>
-    <col min="170" max="170" width="12" customWidth="1"/>
-    <col min="171" max="171" width="3" customWidth="1"/>
-    <col min="172" max="172" width="12" customWidth="1"/>
-    <col min="173" max="173" width="3" customWidth="1"/>
-    <col min="174" max="174" width="12" customWidth="1"/>
-    <col min="175" max="175" width="3" customWidth="1"/>
-    <col min="176" max="176" width="12" customWidth="1"/>
-    <col min="177" max="177" width="3" customWidth="1"/>
-    <col min="178" max="178" width="12" customWidth="1"/>
-    <col min="179" max="179" width="3" customWidth="1"/>
-    <col min="180" max="180" width="12" customWidth="1"/>
-    <col min="181" max="181" width="3" customWidth="1"/>
-    <col min="182" max="182" width="12" customWidth="1"/>
-    <col min="183" max="183" width="3" customWidth="1"/>
-    <col min="184" max="184" width="12" customWidth="1"/>
-    <col min="185" max="185" width="3" customWidth="1"/>
-    <col min="186" max="186" width="12" customWidth="1"/>
-    <col min="187" max="187" width="3" customWidth="1"/>
-    <col min="188" max="188" width="12" customWidth="1"/>
-    <col min="189" max="189" width="3" customWidth="1"/>
-    <col min="190" max="190" width="12" customWidth="1"/>
-    <col min="191" max="191" width="3" customWidth="1"/>
-    <col min="192" max="192" width="12" customWidth="1"/>
-    <col min="193" max="193" width="3" customWidth="1"/>
-    <col min="194" max="194" width="12" customWidth="1"/>
-    <col min="195" max="195" width="3" customWidth="1"/>
-    <col min="196" max="196" width="12" customWidth="1"/>
-    <col min="197" max="197" width="3" customWidth="1"/>
-    <col min="198" max="198" width="12" customWidth="1"/>
-    <col min="199" max="199" width="3" customWidth="1"/>
-    <col min="200" max="200" width="12" customWidth="1"/>
-    <col min="201" max="201" width="22.140625" customWidth="1"/>
-    <col min="202" max="202" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="203" max="203" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="204" max="204" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="2" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="2" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="2" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="14" max="14" width="2" customWidth="1"/>
+    <col min="15" max="15" width="12" customWidth="1"/>
+    <col min="16" max="16" width="2" customWidth="1"/>
+    <col min="17" max="17" width="12" customWidth="1"/>
+    <col min="18" max="18" width="2" customWidth="1"/>
+    <col min="19" max="19" width="12" customWidth="1"/>
+    <col min="20" max="20" width="2" customWidth="1"/>
+    <col min="21" max="21" width="12" customWidth="1"/>
+    <col min="22" max="22" width="3" customWidth="1"/>
+    <col min="23" max="23" width="12" customWidth="1"/>
+    <col min="24" max="24" width="3" customWidth="1"/>
+    <col min="25" max="25" width="12" customWidth="1"/>
+    <col min="26" max="26" width="3" customWidth="1"/>
+    <col min="27" max="27" width="11" customWidth="1"/>
+    <col min="28" max="28" width="3" customWidth="1"/>
+    <col min="29" max="29" width="12" customWidth="1"/>
+    <col min="30" max="30" width="3" customWidth="1"/>
+    <col min="31" max="31" width="10" customWidth="1"/>
+    <col min="32" max="32" width="3" customWidth="1"/>
+    <col min="33" max="33" width="12" customWidth="1"/>
+    <col min="34" max="34" width="3" customWidth="1"/>
+    <col min="35" max="35" width="12" customWidth="1"/>
+    <col min="36" max="36" width="3" customWidth="1"/>
+    <col min="37" max="37" width="12" customWidth="1"/>
+    <col min="38" max="38" width="3" customWidth="1"/>
+    <col min="39" max="39" width="12" customWidth="1"/>
+    <col min="40" max="40" width="3" customWidth="1"/>
+    <col min="41" max="41" width="12" customWidth="1"/>
+    <col min="42" max="42" width="3" customWidth="1"/>
+    <col min="43" max="43" width="12" customWidth="1"/>
+    <col min="44" max="44" width="3" customWidth="1"/>
+    <col min="45" max="45" width="11" customWidth="1"/>
+    <col min="46" max="46" width="3" customWidth="1"/>
+    <col min="47" max="47" width="12" customWidth="1"/>
+    <col min="48" max="48" width="3" customWidth="1"/>
+    <col min="49" max="49" width="12" customWidth="1"/>
+    <col min="50" max="50" width="3" customWidth="1"/>
+    <col min="51" max="51" width="12" customWidth="1"/>
+    <col min="52" max="52" width="3" customWidth="1"/>
+    <col min="53" max="53" width="12" customWidth="1"/>
+    <col min="54" max="54" width="3" customWidth="1"/>
+    <col min="55" max="55" width="12" customWidth="1"/>
+    <col min="56" max="56" width="3" customWidth="1"/>
+    <col min="57" max="57" width="12" customWidth="1"/>
+    <col min="58" max="58" width="3" customWidth="1"/>
+    <col min="59" max="59" width="12" customWidth="1"/>
+    <col min="60" max="60" width="3" customWidth="1"/>
+    <col min="61" max="61" width="12" customWidth="1"/>
+    <col min="62" max="62" width="3" customWidth="1"/>
+    <col min="63" max="63" width="12" customWidth="1"/>
+    <col min="64" max="64" width="3" customWidth="1"/>
+    <col min="65" max="65" width="12" customWidth="1"/>
+    <col min="66" max="66" width="3" customWidth="1"/>
+    <col min="67" max="67" width="12" customWidth="1"/>
+    <col min="68" max="68" width="3" customWidth="1"/>
+    <col min="69" max="69" width="12" customWidth="1"/>
+    <col min="70" max="70" width="3" customWidth="1"/>
+    <col min="71" max="71" width="12" customWidth="1"/>
+    <col min="72" max="72" width="3" customWidth="1"/>
+    <col min="73" max="73" width="12" customWidth="1"/>
+    <col min="74" max="74" width="3" customWidth="1"/>
+    <col min="75" max="75" width="12" customWidth="1"/>
+    <col min="76" max="76" width="3" customWidth="1"/>
+    <col min="77" max="77" width="12" customWidth="1"/>
+    <col min="78" max="78" width="3" customWidth="1"/>
+    <col min="79" max="79" width="12" customWidth="1"/>
+    <col min="80" max="80" width="3" customWidth="1"/>
+    <col min="81" max="81" width="12" customWidth="1"/>
+    <col min="82" max="82" width="3" customWidth="1"/>
+    <col min="83" max="83" width="12" customWidth="1"/>
+    <col min="84" max="84" width="3" customWidth="1"/>
+    <col min="85" max="85" width="11" customWidth="1"/>
+    <col min="86" max="86" width="3" customWidth="1"/>
+    <col min="87" max="87" width="12" customWidth="1"/>
+    <col min="88" max="88" width="3" customWidth="1"/>
+    <col min="89" max="89" width="12" customWidth="1"/>
+    <col min="90" max="90" width="3" customWidth="1"/>
+    <col min="91" max="91" width="11" customWidth="1"/>
+    <col min="92" max="92" width="3" customWidth="1"/>
+    <col min="93" max="93" width="12" customWidth="1"/>
+    <col min="94" max="94" width="3" customWidth="1"/>
+    <col min="95" max="95" width="12" customWidth="1"/>
+    <col min="96" max="96" width="3" customWidth="1"/>
+    <col min="97" max="97" width="12" customWidth="1"/>
+    <col min="98" max="98" width="3" customWidth="1"/>
+    <col min="99" max="99" width="12" customWidth="1"/>
+    <col min="100" max="100" width="3" customWidth="1"/>
+    <col min="101" max="101" width="12" customWidth="1"/>
+    <col min="102" max="102" width="3" customWidth="1"/>
+    <col min="103" max="103" width="12" customWidth="1"/>
+    <col min="104" max="104" width="3" customWidth="1"/>
+    <col min="105" max="105" width="12" customWidth="1"/>
+    <col min="106" max="106" width="3" customWidth="1"/>
+    <col min="107" max="107" width="12" customWidth="1"/>
+    <col min="108" max="108" width="3" customWidth="1"/>
+    <col min="109" max="109" width="12" customWidth="1"/>
+    <col min="110" max="110" width="3" customWidth="1"/>
+    <col min="111" max="111" width="12" customWidth="1"/>
+    <col min="112" max="112" width="3" customWidth="1"/>
+    <col min="113" max="113" width="12" customWidth="1"/>
+    <col min="114" max="114" width="3" customWidth="1"/>
+    <col min="115" max="115" width="12" customWidth="1"/>
+    <col min="116" max="116" width="3" customWidth="1"/>
+    <col min="117" max="117" width="12" customWidth="1"/>
+    <col min="118" max="118" width="3" customWidth="1"/>
+    <col min="119" max="119" width="12" customWidth="1"/>
+    <col min="120" max="120" width="3" customWidth="1"/>
+    <col min="121" max="121" width="12" customWidth="1"/>
+    <col min="122" max="122" width="3" customWidth="1"/>
+    <col min="123" max="123" width="12" customWidth="1"/>
+    <col min="124" max="124" width="3" customWidth="1"/>
+    <col min="125" max="125" width="12" customWidth="1"/>
+    <col min="126" max="126" width="3" customWidth="1"/>
+    <col min="127" max="127" width="12" customWidth="1"/>
+    <col min="128" max="128" width="3" customWidth="1"/>
+    <col min="129" max="129" width="12" customWidth="1"/>
+    <col min="130" max="130" width="3" customWidth="1"/>
+    <col min="131" max="131" width="10" customWidth="1"/>
+    <col min="132" max="132" width="3" customWidth="1"/>
+    <col min="133" max="133" width="12" customWidth="1"/>
+    <col min="134" max="134" width="3" customWidth="1"/>
+    <col min="135" max="135" width="12" customWidth="1"/>
+    <col min="136" max="136" width="3" customWidth="1"/>
+    <col min="137" max="137" width="12" customWidth="1"/>
+    <col min="138" max="138" width="3" customWidth="1"/>
+    <col min="139" max="139" width="12" customWidth="1"/>
+    <col min="140" max="140" width="3" customWidth="1"/>
+    <col min="141" max="141" width="12" customWidth="1"/>
+    <col min="142" max="142" width="3" customWidth="1"/>
+    <col min="143" max="143" width="12" customWidth="1"/>
+    <col min="144" max="144" width="3" customWidth="1"/>
+    <col min="145" max="145" width="12" customWidth="1"/>
+    <col min="146" max="146" width="3" customWidth="1"/>
+    <col min="147" max="147" width="12" customWidth="1"/>
+    <col min="148" max="148" width="3" customWidth="1"/>
+    <col min="149" max="149" width="12" customWidth="1"/>
+    <col min="150" max="150" width="3" customWidth="1"/>
+    <col min="151" max="151" width="12" customWidth="1"/>
+    <col min="152" max="152" width="3" customWidth="1"/>
+    <col min="153" max="153" width="12" customWidth="1"/>
+    <col min="154" max="154" width="3" customWidth="1"/>
+    <col min="155" max="155" width="12" customWidth="1"/>
+    <col min="156" max="156" width="3" customWidth="1"/>
+    <col min="157" max="157" width="12" customWidth="1"/>
+    <col min="158" max="158" width="3" customWidth="1"/>
+    <col min="159" max="159" width="12" customWidth="1"/>
+    <col min="160" max="160" width="3" customWidth="1"/>
+    <col min="161" max="161" width="12" customWidth="1"/>
+    <col min="162" max="162" width="3" customWidth="1"/>
+    <col min="163" max="163" width="12" customWidth="1"/>
+    <col min="164" max="164" width="3" customWidth="1"/>
+    <col min="165" max="165" width="12" customWidth="1"/>
+    <col min="166" max="166" width="3" customWidth="1"/>
+    <col min="167" max="167" width="12" customWidth="1"/>
+    <col min="168" max="168" width="3" customWidth="1"/>
+    <col min="169" max="169" width="12" customWidth="1"/>
+    <col min="170" max="170" width="3" customWidth="1"/>
+    <col min="171" max="171" width="12" customWidth="1"/>
+    <col min="172" max="172" width="3" customWidth="1"/>
+    <col min="173" max="173" width="12" customWidth="1"/>
+    <col min="174" max="174" width="3" customWidth="1"/>
+    <col min="175" max="175" width="12" customWidth="1"/>
+    <col min="176" max="176" width="3" customWidth="1"/>
+    <col min="177" max="177" width="12" customWidth="1"/>
+    <col min="178" max="178" width="3" customWidth="1"/>
+    <col min="179" max="179" width="12" customWidth="1"/>
+    <col min="180" max="180" width="3" customWidth="1"/>
+    <col min="181" max="181" width="12" customWidth="1"/>
+    <col min="182" max="182" width="3" customWidth="1"/>
+    <col min="183" max="183" width="12" customWidth="1"/>
+    <col min="184" max="184" width="3" customWidth="1"/>
+    <col min="185" max="185" width="12" customWidth="1"/>
+    <col min="186" max="186" width="3" customWidth="1"/>
+    <col min="187" max="187" width="12" customWidth="1"/>
+    <col min="188" max="188" width="3" customWidth="1"/>
+    <col min="189" max="189" width="12" customWidth="1"/>
+    <col min="190" max="190" width="3" customWidth="1"/>
+    <col min="191" max="191" width="12" customWidth="1"/>
+    <col min="192" max="192" width="3" customWidth="1"/>
+    <col min="193" max="193" width="12" customWidth="1"/>
+    <col min="194" max="194" width="3" customWidth="1"/>
+    <col min="195" max="195" width="12" customWidth="1"/>
+    <col min="196" max="196" width="3" customWidth="1"/>
+    <col min="197" max="197" width="12" customWidth="1"/>
+    <col min="198" max="198" width="3" customWidth="1"/>
+    <col min="199" max="199" width="12" customWidth="1"/>
+    <col min="200" max="200" width="3" customWidth="1"/>
+    <col min="201" max="201" width="12" customWidth="1"/>
+    <col min="202" max="202" width="22.140625" customWidth="1"/>
+    <col min="203" max="203" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="204" max="204" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="205" max="205" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -618,802 +620,802 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>6.1407105587742896E-3</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>6.5682566510815096E-3</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>71</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>4.0242211524544297E-2</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>4.3734007040873699E-2</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>5.6527166628966598E-2</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>93</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>8.3782366815788795E-2</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>9.3471082326174099E-2</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>0.10308439182415099</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>0.107688649539867</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>0.11361578745629899</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>0.114935625988989</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>0.122516248867388</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>0.13154273935875799</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
-        <v>98</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>0.141189123151094</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>0.149320990805445</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>0.15260639389269101</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>0.166626924552704</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>0.16708381429445901</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>0.180280464537625</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>0.191176268514824</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>0.20788485398599699</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>0.215648305817532</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>78</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>0.21882513885659499</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>0.23468203964763201</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>0.23760475051573701</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>0.24272335546106499</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>0.27525282040250498</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>0.29632546946889299</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>82</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>0.31525008084226502</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>0.32790130098310999</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>0.337277468013991</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>0.33851172994047601</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>0.35014379649940902</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B35">
-        <v>0.35389694449786602</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36">
-        <v>28</v>
-      </c>
-      <c r="B36">
-        <v>0.36136692037587798</v>
+        <v>34</v>
+      </c>
+      <c r="B36" s="1">
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>0.36660280396287798</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38">
-        <v>62</v>
-      </c>
-      <c r="B38">
-        <v>0.37064518594002399</v>
+        <v>36</v>
+      </c>
+      <c r="B38" s="1">
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="B39">
-        <v>0.37184849115489799</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>0.37313247347568901</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="B41">
-        <v>0.38273996169003399</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="B42">
-        <v>0.40131083610893897</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="B43">
-        <v>0.41391193026385797</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B44">
-        <v>0.41678837115846301</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="B45">
-        <v>0.42477069907861398</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="B46">
-        <v>0.43918420682217202</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47">
-        <v>0.44421191475670102</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B48">
-        <v>0.46818206324168998</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B49">
-        <v>0.496221285028492</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="B50">
-        <v>0.49703090985797699</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="B51">
-        <v>0.502974753449691</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B52">
-        <v>0.51060013690083295</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="B53">
-        <v>0.51335735362388202</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B54">
-        <v>0.52060333759657496</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="B55">
-        <v>0.54795469822383902</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="B56">
-        <v>0.56944167023091197</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="B57">
-        <v>0.57299285517202703</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B58">
-        <v>0.59503402476128897</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B59">
-        <v>0.60406331605611996</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="B60">
-        <v>0.61972255026799905</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="B61">
-        <v>0.628520653306336</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B62">
-        <v>0.657413411108973</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B63">
-        <v>0.66010583556945301</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B64">
-        <v>0.66844738940857795</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="B65">
-        <v>0.68929623579575205</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B66">
-        <v>0.69502900054819094</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="B67">
-        <v>0.69631870084979097</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B68">
-        <v>0.69918173381858095</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B69">
-        <v>0.70209656555820299</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="B70">
-        <v>0.70309928475577599</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="B71">
-        <v>0.70398715764507402</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B72">
-        <v>0.72440986154035103</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="B73">
-        <v>0.73671229765734003</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B74">
-        <v>0.74491525602084796</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="B75">
-        <v>0.75030559403655495</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="B76">
-        <v>0.75036001051109802</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B77">
-        <v>0.75404839444098803</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B78">
-        <v>0.75784349910094295</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="B79">
-        <v>0.76708642307281205</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="B80">
-        <v>0.77082135373875804</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="B81">
-        <v>0.77686734734025698</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="B82">
-        <v>0.78721848409506001</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="B83">
-        <v>0.79286486895467501</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="B84">
-        <v>0.80862034919647097</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="B85">
-        <v>0.81121187689277696</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B86">
-        <v>0.82637894166165304</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="B87">
-        <v>0.84095621107352903</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="B88">
-        <v>0.86023351341491705</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="B89">
-        <v>0.86510707324816605</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="B90">
-        <v>0.87383680891213</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="B91">
-        <v>0.88468112587043501</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="B92">
-        <v>0.88588497427844703</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="B93">
-        <v>0.90322732391725202</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="B94">
-        <v>0.91099547880238096</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="B95">
-        <v>0.93687062924168096</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="B96">
-        <v>0.94333347974172399</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="B97">
-        <v>0.952245347626685</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B98">
-        <v>0.96108955748244596</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B99">
-        <v>0.96123722551180002</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="B100">
-        <v>0.97483728148725701</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="B101">
-        <v>0.97761793868570701</v>
+        <v>6.4936520277775103E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add comments to abstain files
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -626,420 +626,420 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="B2">
-        <v>0.37356957174234401</v>
+        <v>0.97492344369863104</v>
       </c>
       <c r="C2">
-        <v>3.74381871629655E-2</v>
+        <v>0.25789701193273901</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="B3">
-        <v>0.111134418961968</v>
+        <v>0.97422420020359202</v>
       </c>
       <c r="C3">
-        <v>0.25074106757887599</v>
+        <v>0.85539968502074903</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B4">
-        <v>0.61121318206040698</v>
+        <v>0.94590240255402303</v>
       </c>
       <c r="C4">
-        <v>0.61171084023675504</v>
+        <v>0.28727535177932201</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="B5">
-        <v>0.31864687570973999</v>
+        <v>0.938257587706679</v>
       </c>
       <c r="C5">
-        <v>0.55505508591738395</v>
+        <v>0.35036249099341898</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="B6">
-        <v>0.56340343145683802</v>
+        <v>0.931918684484078</v>
       </c>
       <c r="C6">
-        <v>0.88901794128391698</v>
+        <v>0.39804241554148301</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B7">
-        <v>0.93632309422276105</v>
+        <v>0.931270998672733</v>
       </c>
       <c r="C7">
-        <v>0.59104858322712295</v>
+        <v>0.82871565479643094</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="B8">
-        <v>0.14358893692548599</v>
+        <v>0.92176562148661501</v>
       </c>
       <c r="C8">
-        <v>0.82697443505456403</v>
+        <v>0.43301052465230599</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="B9">
-        <v>0.116632876148761</v>
+        <v>0.89881671768124105</v>
       </c>
       <c r="C9">
-        <v>0.74800041269181905</v>
+        <v>0.91556051357701895</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B10">
-        <v>0.66298307562077397</v>
+        <v>0.82833793417917201</v>
       </c>
       <c r="C10">
-        <v>0.41483787736042599</v>
+        <v>0.93632287594027197</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>9</v>
+        <v>89</v>
       </c>
       <c r="B11">
-        <v>0.965423813394373</v>
+        <v>0.81349507460942305</v>
       </c>
       <c r="C11">
-        <v>0.29417691614924302</v>
+        <v>0.179848870481018</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="B12">
-        <v>0.77330773360272198</v>
+        <v>0.81251708077597595</v>
       </c>
       <c r="C12">
-        <v>0.14342165918684199</v>
+        <v>0.18657992941648499</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="B13">
-        <v>0.60460059829454804</v>
+        <v>0.79785439724937801</v>
       </c>
       <c r="C13">
-        <v>0.74674386702270101</v>
+        <v>0.74265455063774899</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B14">
-        <v>0.116632876148761</v>
+        <v>0.79261030206501404</v>
       </c>
       <c r="C14">
-        <v>0.74800041269181905</v>
+        <v>0.94957770108051598</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="B15">
-        <v>0.87547323806341604</v>
+        <v>0.79236264357230601</v>
       </c>
       <c r="C15">
-        <v>1.7361499046249201E-2</v>
+        <v>0.72416091593012299</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="B16">
-        <v>0.116632876148761</v>
+        <v>0.79153473221170401</v>
       </c>
       <c r="C16">
-        <v>0.74800041269181905</v>
+        <v>0.61542450401362503</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>5.9797910802554803E-2</v>
+        <v>98</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.76375210997500997</v>
       </c>
       <c r="C17">
-        <v>0.48781128929405398</v>
+        <v>0.54898203033125004</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B18">
-        <v>0.111134418961968</v>
+        <v>0.757281704178419</v>
       </c>
       <c r="C18">
-        <v>0.25074106757887599</v>
+        <v>0.88495877963068204</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="B19">
-        <v>0.214435583502221</v>
+        <v>0.75378441523307105</v>
       </c>
       <c r="C19">
-        <v>0.97178396433032999</v>
+        <v>0.53755819541862404</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B20">
-        <v>5.29419226968076E-2</v>
+        <v>0.73598923955831697</v>
       </c>
       <c r="C20">
-        <v>0.54728143696990394</v>
+        <v>0.16273186564763401</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B21">
-        <v>0.56989071888225495</v>
+        <v>0.73518703179911105</v>
       </c>
       <c r="C21">
-        <v>0.77633783964689096</v>
+        <v>4.6395229592129598E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B22">
-        <v>0.92329668809050702</v>
+        <v>0.71781631747118302</v>
       </c>
       <c r="C22">
-        <v>0.63318052885891496</v>
+        <v>0.418010229504163</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B23">
-        <v>0.87956363109244295</v>
+        <v>0.71491115012532003</v>
       </c>
       <c r="C23">
-        <v>0.83628181218596798</v>
+        <v>0.331903672719427</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="B24">
-        <v>0.27617100837175701</v>
+        <v>0.70270876588616205</v>
       </c>
       <c r="C24">
-        <v>0.76172711459098696</v>
+        <v>1.69909910621821E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B25">
-        <v>0.65869004674757403</v>
+        <v>0.70097148276211296</v>
       </c>
       <c r="C25">
-        <v>0.45218837517120403</v>
+        <v>0.80697005386595699</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B26">
-        <v>0.76535881164716701</v>
+        <v>0.68679320536493504</v>
       </c>
       <c r="C26">
-        <v>0.85238921022017999</v>
+        <v>0.94880681758879204</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="B27">
-        <v>0.99636011621430698</v>
+        <v>0.67159190043856198</v>
       </c>
       <c r="C27">
-        <v>0.53056640184499204</v>
+        <v>0.42173231578016601</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="B28">
-        <v>0.89222895151730297</v>
+        <v>0.66076887478680701</v>
       </c>
       <c r="C28">
-        <v>0.62106306430569602</v>
+        <v>0.63660184948133502</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B29">
-        <v>0.22109860788608199</v>
+        <v>0.63494420296593701</v>
       </c>
       <c r="C29">
-        <v>6.7602626035270896E-2</v>
+        <v>0.811772726695146</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="B30">
-        <v>0.82160842911078003</v>
+        <v>0.61923706568047998</v>
       </c>
       <c r="C30">
-        <v>6.0059957365813599E-2</v>
+        <v>0.26691372497690102</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B31">
-        <v>0.95524161937211705</v>
+        <v>0.61923706568047998</v>
       </c>
       <c r="C31">
-        <v>0.17023398239576101</v>
+        <v>0.26691372497690102</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B32">
-        <v>0.80304142127918199</v>
+        <v>0.61923706568047998</v>
       </c>
       <c r="C32">
-        <v>0.75802716849927598</v>
+        <v>0.26691372497690102</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>31</v>
+        <v>94</v>
       </c>
       <c r="B33">
-        <v>0.30134152175976098</v>
+        <v>0.61923706568047998</v>
       </c>
       <c r="C33">
-        <v>0.74689699439775503</v>
+        <v>0.26691372497690102</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="B34">
-        <v>0.64980306238181096</v>
+        <v>0.60614127712016097</v>
       </c>
       <c r="C34">
-        <v>0.90687882199919301</v>
+        <v>0.69652675863931002</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B35">
-        <v>0.37356957174234401</v>
+        <v>0.60024200639661496</v>
       </c>
       <c r="C35">
-        <v>3.74381871629655E-2</v>
+        <v>7.3245617998138501E-2</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="B36">
-        <v>0.820367280406333</v>
+        <v>0.599362936916089</v>
       </c>
       <c r="C36">
-        <v>0.273549110220633</v>
+        <v>0.92834609269282897</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="B37">
-        <v>0.147948535889591</v>
+        <v>0.596964868281185</v>
       </c>
       <c r="C37">
-        <v>0.14141483655131701</v>
+        <v>0.17416469003545099</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="B38">
-        <v>0.56635426748361495</v>
+        <v>0.59337304247759803</v>
       </c>
       <c r="C38">
-        <v>0.87296329470508005</v>
+        <v>0.75245492589179297</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B39">
-        <v>0.88550722923323499</v>
+        <v>0.58780330025065697</v>
       </c>
       <c r="C39">
-        <v>0.610470654162374</v>
+        <v>0.93396899609456596</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1047,681 +1047,681 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0.97881397134166903</v>
+        <v>0.58696803697710698</v>
       </c>
       <c r="C40">
-        <v>0.41991575038157097</v>
+        <v>0.68720126458175201</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B41">
-        <v>0.58243335753327796</v>
+        <v>0.576867934730242</v>
       </c>
       <c r="C41">
-        <v>0.54621966471820105</v>
+        <v>0.78676015328792104</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="B42">
-        <v>0.59804431258225499</v>
+        <v>0.55965033314593504</v>
       </c>
       <c r="C42">
-        <v>0.84488464007469999</v>
+        <v>0.78698655955783703</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B43">
-        <v>0.92383313015152002</v>
+        <v>0.55949911671065999</v>
       </c>
       <c r="C43">
-        <v>0.97944140431358095</v>
+        <v>0.99243671472129302</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="B44">
-        <v>0.86214824219195196</v>
+        <v>0.55089526203750605</v>
       </c>
       <c r="C44">
-        <v>0.96495252770642403</v>
+        <v>0.69583286195467897</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="B45">
-        <v>0.226458707082693</v>
+        <v>0.54581173532131799</v>
       </c>
       <c r="C45">
-        <v>0.18545162896116099</v>
+        <v>0.57033125633842396</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B46">
-        <v>0.90160137362045301</v>
+        <v>0.50267877809991102</v>
       </c>
       <c r="C46">
-        <v>0.89235029858169002</v>
+        <v>0.52884593508329403</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B47">
-        <v>0.39666966217308097</v>
+        <v>0.48795119906801598</v>
       </c>
       <c r="C47">
-        <v>0.142141284408388</v>
+        <v>0.81031639436515901</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="B48">
-        <v>1.0504707884239E-2</v>
+        <v>0.48191526048989802</v>
       </c>
       <c r="C48">
-        <v>0.13099380005935299</v>
+        <v>6.3064960665017794E-2</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B49">
-        <v>0.78642050623227899</v>
+        <v>0.47851964762430699</v>
       </c>
       <c r="C49">
-        <v>0.92745871329801499</v>
+        <v>0.53302450459772599</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B50">
-        <v>0.12024059030658001</v>
+        <v>0.47851964762430699</v>
       </c>
       <c r="C50">
-        <v>0.45725267245373702</v>
+        <v>0.53302450459772599</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="B51">
-        <v>3.8515562192165099E-3</v>
+        <v>0.46446538069166099</v>
       </c>
       <c r="C51">
-        <v>0.831672896517895</v>
+        <v>0.42829806740164</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B52">
-        <v>0.116632876148761</v>
+        <v>0.430012167353374</v>
       </c>
       <c r="C52">
-        <v>0.74800041269181905</v>
+        <v>0.884860324990001</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="B53">
-        <v>0.984559763341187</v>
+        <v>0.42150366669794498</v>
       </c>
       <c r="C53">
-        <v>0.325713361009557</v>
+        <v>0.222755918991172</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="B54">
-        <v>0.93423217501843803</v>
+        <v>0.42150366669794498</v>
       </c>
       <c r="C54">
-        <v>0.37076507349451598</v>
+        <v>0.222755918991172</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="B55">
-        <v>0.95188072077196895</v>
+        <v>0.42150366669794498</v>
       </c>
       <c r="C55">
-        <v>0.91361844088441302</v>
+        <v>0.222755918991172</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B56">
-        <v>0.49319486919509198</v>
+        <v>0.42150366669794498</v>
       </c>
       <c r="C56">
-        <v>0.62406898869734195</v>
+        <v>0.222755918991172</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="B57">
-        <v>7.3122832688726894E-2</v>
+        <v>0.38879122559795398</v>
       </c>
       <c r="C57">
-        <v>0.618997493968656</v>
+        <v>0.45355088553567302</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="B58">
-        <v>0.28958620764075199</v>
+        <v>0.37644437855021801</v>
       </c>
       <c r="C58">
-        <v>0.37283202501728602</v>
+        <v>0.80977490532521801</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B59">
-        <v>0.44160948620222501</v>
+        <v>0.37441526147772197</v>
       </c>
       <c r="C59">
-        <v>0.70532817714178897</v>
+        <v>1.9728734871265999E-3</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B60">
-        <v>0.87403847909390897</v>
+        <v>0.36909321613217</v>
       </c>
       <c r="C60">
-        <v>0.49016972202084502</v>
+        <v>0.94582865395905302</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="B61">
-        <v>0.344571771049551</v>
+        <v>0.36184962079489902</v>
       </c>
       <c r="C61">
-        <v>0.35558790351587699</v>
+        <v>1.5951822834761899E-2</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="B62">
-        <v>0.34447997455987101</v>
+        <v>0.36184962079489902</v>
       </c>
       <c r="C62">
-        <v>0.21604457940534499</v>
+        <v>1.5951822834761899E-2</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B63">
-        <v>3.7099338954616201E-2</v>
+        <v>0.36184962079489902</v>
       </c>
       <c r="C63">
-        <v>0.41843551862695499</v>
+        <v>1.5951822834761899E-2</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="B64">
-        <v>0.37356957174234401</v>
+        <v>0.35317473883684902</v>
       </c>
       <c r="C64">
-        <v>3.74381871629655E-2</v>
+        <v>0.605677549132281</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="B65">
-        <v>0.52224468286140902</v>
+        <v>0.33725842914849202</v>
       </c>
       <c r="C65">
-        <v>0.85396570411347805</v>
+        <v>0.76944558082588999</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="B66">
-        <v>0.36830529021564201</v>
+        <v>0.32966043923215799</v>
       </c>
       <c r="C66">
-        <v>0.46458038023117099</v>
+        <v>0.179670244936292</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B67">
-        <v>0.77473355084940998</v>
+        <v>0.32937756315966799</v>
       </c>
       <c r="C67">
-        <v>9.6246775342462204E-2</v>
+        <v>0.12875489542062099</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68">
-        <v>66</v>
-      </c>
-      <c r="B68">
-        <v>0.24173598909938601</v>
+        <v>70</v>
+      </c>
+      <c r="B68" s="1">
+        <v>0.32849934894517502</v>
       </c>
       <c r="C68">
-        <v>0.94051062428800902</v>
+        <v>0.417730337267125</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B69">
-        <v>0.55648686646913703</v>
+        <v>0.32695083644963602</v>
       </c>
       <c r="C69">
-        <v>0.45305538812130802</v>
+        <v>0.46898738146291102</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="B70">
-        <v>0.95384204785844795</v>
+        <v>0.32454977147685798</v>
       </c>
       <c r="C70">
-        <v>9.8742596686744594E-2</v>
+        <v>1.9622903041966001E-2</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="B71">
-        <v>0.37356957174234401</v>
+        <v>0.31131117566531502</v>
       </c>
       <c r="C71">
-        <v>3.74381871629655E-2</v>
+        <v>2.0756162848575E-2</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72">
-        <v>70</v>
-      </c>
-      <c r="B72" s="1">
-        <v>0.97691031891170299</v>
+        <v>25</v>
+      </c>
+      <c r="B72">
+        <v>0.305065050262884</v>
       </c>
       <c r="C72">
-        <v>0.299890596685708</v>
+        <v>0.26464738226225898</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="B73">
-        <v>0.87179420946570996</v>
+        <v>0.30104169043092399</v>
       </c>
       <c r="C73">
-        <v>0.55540129495297497</v>
+        <v>0.227658343138399</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="B74">
-        <v>1.52330042349263E-2</v>
+        <v>0.285576193261875</v>
       </c>
       <c r="C74">
-        <v>9.1581009558242693E-2</v>
+        <v>0.249542249261717</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="B75">
-        <v>0.24588493072005599</v>
+        <v>0.27311053697450199</v>
       </c>
       <c r="C75">
-        <v>0.410760042231537</v>
+        <v>0.96098124753941505</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="B76">
-        <v>0.57375627224292602</v>
+        <v>0.27216523108002499</v>
       </c>
       <c r="C76">
-        <v>0.95500066150611695</v>
+        <v>0.56746021189958196</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B77">
-        <v>0.94666497800444704</v>
+        <v>0.26922808056090702</v>
       </c>
       <c r="C77">
-        <v>0.73271207104010905</v>
+        <v>0.72908519542272399</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="B78">
-        <v>0.61266911331803298</v>
+        <v>0.25985428860168203</v>
       </c>
       <c r="C78">
-        <v>0.53984782357863703</v>
+        <v>0.96044720984480303</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B79">
-        <v>0.32903313632425202</v>
+        <v>0.234324443370894</v>
       </c>
       <c r="C79">
-        <v>0.34145641285754702</v>
+        <v>0.86389825205075199</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80">
-        <v>78</v>
+        <v>10</v>
       </c>
       <c r="B80">
-        <v>0.209122928048325</v>
+        <v>0.18686320236439199</v>
       </c>
       <c r="C80">
-        <v>0.21859093939185401</v>
+        <v>0.92313482652757395</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="B81">
-        <v>0.54261565098164299</v>
+        <v>0.17666646878884601</v>
       </c>
       <c r="C81">
-        <v>0.74245906986245602</v>
+        <v>0.18844246436734199</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="B82">
-        <v>0.95282309033256296</v>
+        <v>0.172211683408036</v>
       </c>
       <c r="C82">
-        <v>0.77124022714638496</v>
+        <v>0.81756740846442499</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="B83">
-        <v>0.71820337190707195</v>
+        <v>0.16379535000342599</v>
       </c>
       <c r="C83">
-        <v>0.636594307066781</v>
+        <v>0.43990456107967202</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="B84">
-        <v>0.31906745225085897</v>
+        <v>0.15001692792260299</v>
       </c>
       <c r="C84">
-        <v>0.52215409637657295</v>
+        <v>0.55149636499285404</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B85">
-        <v>0.20214286406172299</v>
+        <v>0.134132935900411</v>
       </c>
       <c r="C85">
-        <v>0.242275725127684</v>
+        <v>0.977784004744785</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B86">
-        <v>0.378015445546942</v>
+        <v>0.122572070493049</v>
       </c>
       <c r="C86">
-        <v>0.74549803211879495</v>
+        <v>0.39976280768397998</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87">
-        <v>85</v>
+        <v>46</v>
       </c>
       <c r="B87">
-        <v>0.23522027306874299</v>
+        <v>0.117020382718869</v>
       </c>
       <c r="C87">
-        <v>0.22753839799355899</v>
+        <v>0.40940448452717199</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B88">
-        <v>0.17017372947170101</v>
+        <v>0.117020382718869</v>
       </c>
       <c r="C88">
-        <v>0.17345507353376799</v>
+        <v>0.40940448452717199</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B89">
-        <v>0.63088324098748005</v>
+        <v>0.114918844520482</v>
       </c>
       <c r="C89">
-        <v>0.16944497235394301</v>
+        <v>0.76592030864147598</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="B90">
-        <v>0.261736627357676</v>
+        <v>9.8624063476444201E-2</v>
       </c>
       <c r="C90">
-        <v>0.42728562717957502</v>
+        <v>0.54585946710943001</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="B91">
-        <v>0.111134418961968</v>
+        <v>9.1716595007661494E-2</v>
       </c>
       <c r="C91">
-        <v>0.25074106757887599</v>
+        <v>0.84914421244191596</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B92">
-        <v>0.98973452525362404</v>
+        <v>8.7514057967843506E-2</v>
       </c>
       <c r="C92">
-        <v>1.72542197223137E-2</v>
+        <v>0.67504053390338403</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="B93">
-        <v>0.688157746564243</v>
+        <v>8.3168022991189403E-2</v>
       </c>
       <c r="C93">
-        <v>0.30499589932860099</v>
+        <v>0.88767906402437802</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B94">
-        <v>0.337284338702664</v>
+        <v>7.0998858178492705E-2</v>
       </c>
       <c r="C94">
-        <v>0.24251363440016399</v>
+        <v>0.55739630908420301</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="B95">
-        <v>0.69032273002489197</v>
+        <v>5.9800329900558599E-2</v>
       </c>
       <c r="C95">
-        <v>0.37903728093253702</v>
+        <v>0.89613977539746104</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="B96">
-        <v>7.4848545722318305E-2</v>
+        <v>5.5365282412294201E-2</v>
       </c>
       <c r="C96">
-        <v>0.76960334341371095</v>
+        <v>0.10127765123867501</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="B97">
-        <v>0.55063580337191498</v>
+        <v>4.6296895400565002E-2</v>
       </c>
       <c r="C97">
-        <v>0.241764648234082</v>
+        <v>1.1404768794402199E-2</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="B98">
-        <v>0.19129752702729799</v>
+        <v>4.6296895400565002E-2</v>
       </c>
       <c r="C98">
-        <v>0.66806539464714099</v>
+        <v>1.1404768794402199E-2</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="B99">
-        <v>0.71847782229922597</v>
+        <v>4.4269185249727297E-2</v>
       </c>
       <c r="C99">
-        <v>0.81083299379181795</v>
+        <v>0.764303486389598</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100">
-        <v>98</v>
-      </c>
-      <c r="B100" s="1">
-        <v>2.9530316069427E-2</v>
+        <v>3</v>
+      </c>
+      <c r="B100">
+        <v>1.8331808375969299E-2</v>
       </c>
       <c r="C100">
-        <v>0.69419288473349905</v>
+        <v>0.45297667443607997</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101">
-        <v>99</v>
-      </c>
-      <c r="B101">
-        <v>0.68805229207083995</v>
+        <v>73</v>
+      </c>
+      <c r="B101" s="1">
+        <v>2.7403684536631001E-4</v>
       </c>
       <c r="C101">
-        <v>0.51848977574611499</v>
+        <v>0.820503462613421</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add AbstainSpatialEvoUG3 and new square grid visualisation method
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -51,10 +51,10 @@
     <t>q</t>
   </si>
   <si>
-    <t>Program: AbstainEvoUG1</t>
+    <t>Gens: 10000</t>
   </si>
   <si>
-    <t>Gens: 100000</t>
+    <t>Program: AbstainSpatialEvoUG3</t>
   </si>
 </sst>
 </file>
@@ -393,14 +393,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.42578125" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
@@ -615,10 +617,10 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -626,24 +628,24 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="B2">
-        <v>0.97492344369863104</v>
+        <v>0.22708802806103201</v>
       </c>
       <c r="C2">
-        <v>0.25789701193273901</v>
+        <v>0.25985848290028302</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="B3">
-        <v>0.97422420020359202</v>
+        <v>0.228354910873624</v>
       </c>
       <c r="C3">
-        <v>0.85539968502074903</v>
+        <v>0.244272475747462</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -651,439 +653,439 @@
         <v>36</v>
       </c>
       <c r="B4">
-        <v>0.94590240255402303</v>
+        <v>0.25201310538343402</v>
       </c>
       <c r="C4">
-        <v>0.28727535177932201</v>
+        <v>0.24005547799299501</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="B5">
-        <v>0.938257587706679</v>
+        <v>0.16027441668659401</v>
       </c>
       <c r="C5">
-        <v>0.35036249099341898</v>
+        <v>0.23439807253009401</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B6">
-        <v>0.931918684484078</v>
+        <v>0.202826846489227</v>
       </c>
       <c r="C6">
-        <v>0.39804241554148301</v>
+        <v>0.22766223774542699</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="B7">
-        <v>0.931270998672733</v>
+        <v>0.15487477267167701</v>
       </c>
       <c r="C7">
-        <v>0.82871565479643094</v>
+        <v>0.220810158492904</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>84</v>
-      </c>
-      <c r="B8">
-        <v>0.92176562148661501</v>
+        <v>12</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.229075061227381</v>
       </c>
       <c r="C8">
-        <v>0.43301052465230599</v>
+        <v>0.22038318859047201</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="B9">
-        <v>0.89881671768124105</v>
+        <v>0.21818033892341801</v>
       </c>
       <c r="C9">
-        <v>0.91556051357701895</v>
+        <v>0.21699014808572401</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="B10">
-        <v>0.82833793417917201</v>
+        <v>9.2952982609301099E-2</v>
       </c>
       <c r="C10">
-        <v>0.93632287594027197</v>
+        <v>0.21518048747583499</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="B11">
-        <v>0.81349507460942305</v>
+        <v>0.25631368519651199</v>
       </c>
       <c r="C11">
-        <v>0.179848870481018</v>
+        <v>0.199001935251336</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B12">
-        <v>0.81251708077597595</v>
+        <v>0.25943777193821899</v>
       </c>
       <c r="C12">
-        <v>0.18657992941648499</v>
+        <v>0.188620515813467</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>0.79785439724937801</v>
+        <v>0.13344974327415099</v>
       </c>
       <c r="C13">
-        <v>0.74265455063774899</v>
+        <v>0.17402979079098799</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B14">
-        <v>0.79261030206501404</v>
+        <v>0.37482507189002701</v>
       </c>
       <c r="C14">
-        <v>0.94957770108051598</v>
+        <v>0.166676423564699</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15">
-        <v>91</v>
+        <v>22</v>
       </c>
       <c r="B15">
-        <v>0.79236264357230601</v>
+        <v>0.18176492785178899</v>
       </c>
       <c r="C15">
-        <v>0.72416091593012299</v>
+        <v>0.164171033481921</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="B16">
-        <v>0.79153473221170401</v>
+        <v>0.18995579720761199</v>
       </c>
       <c r="C16">
-        <v>0.61542450401362503</v>
+        <v>0.16331051047825901</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>98</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0.76375210997500997</v>
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>0.209358271755412</v>
       </c>
       <c r="C17">
-        <v>0.54898203033125004</v>
+        <v>0.160361498240888</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="B18">
-        <v>0.757281704178419</v>
+        <v>7.3087205426551505E-2</v>
       </c>
       <c r="C18">
-        <v>0.88495877963068204</v>
+        <v>0.160187243696267</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="B19">
-        <v>0.75378441523307105</v>
+        <v>0.159124948024394</v>
       </c>
       <c r="C19">
-        <v>0.53755819541862404</v>
+        <v>0.15534428029123301</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="B20">
-        <v>0.73598923955831697</v>
+        <v>0.162779874696935</v>
       </c>
       <c r="C20">
-        <v>0.16273186564763401</v>
+        <v>0.154145121202927</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B21">
-        <v>0.73518703179911105</v>
+        <v>0.19405821240914101</v>
       </c>
       <c r="C21">
-        <v>4.6395229592129598E-2</v>
+        <v>0.15261110929442001</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="B22">
-        <v>0.71781631747118302</v>
+        <v>0.13547796896327099</v>
       </c>
       <c r="C22">
-        <v>0.418010229504163</v>
+        <v>0.15011215281656801</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B23">
-        <v>0.71491115012532003</v>
+        <v>0.21771070400426301</v>
       </c>
       <c r="C23">
-        <v>0.331903672719427</v>
+        <v>0.14559576689682599</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="B24">
-        <v>0.70270876588616205</v>
+        <v>0.138624019928722</v>
       </c>
       <c r="C24">
-        <v>1.69909910621821E-2</v>
+        <v>0.143992014309027</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B25">
-        <v>0.70097148276211296</v>
+        <v>0.23184152473448</v>
       </c>
       <c r="C25">
-        <v>0.80697005386595699</v>
+        <v>0.142791447947344</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B26">
-        <v>0.68679320536493504</v>
+        <v>0.274815443258832</v>
       </c>
       <c r="C26">
-        <v>0.94880681758879204</v>
+        <v>0.14187590122088101</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B27">
-        <v>0.67159190043856198</v>
+        <v>9.6435915128152194E-2</v>
       </c>
       <c r="C27">
-        <v>0.42173231578016601</v>
+        <v>0.13526410214850901</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="B28">
-        <v>0.66076887478680701</v>
+        <v>0.104069314809717</v>
       </c>
       <c r="C28">
-        <v>0.63660184948133502</v>
+        <v>0.133793415949918</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="B29">
-        <v>0.63494420296593701</v>
+        <v>9.5296144266763094E-3</v>
       </c>
       <c r="C29">
-        <v>0.811772726695146</v>
+        <v>0.13319141781108801</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B30">
-        <v>0.61923706568047998</v>
+        <v>0.134698105127598</v>
       </c>
       <c r="C30">
-        <v>0.26691372497690102</v>
+        <v>0.13206628661175501</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="B31">
-        <v>0.61923706568047998</v>
+        <v>0.367862139060398</v>
       </c>
       <c r="C31">
-        <v>0.26691372497690102</v>
+        <v>0.12781208346621301</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B32">
-        <v>0.61923706568047998</v>
+        <v>0.191210557968957</v>
       </c>
       <c r="C32">
-        <v>0.26691372497690102</v>
+        <v>0.123754150737308</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>94</v>
+        <v>46</v>
       </c>
       <c r="B33">
-        <v>0.61923706568047998</v>
+        <v>0.43016484882846301</v>
       </c>
       <c r="C33">
-        <v>0.26691372497690102</v>
+        <v>0.1237409559967</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B34">
-        <v>0.60614127712016097</v>
+        <v>0.26043207732158102</v>
       </c>
       <c r="C34">
-        <v>0.69652675863931002</v>
+        <v>0.12084683561479399</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B35">
-        <v>0.60024200639661496</v>
+        <v>0.34022411813074399</v>
       </c>
       <c r="C35">
-        <v>7.3245617998138501E-2</v>
+        <v>0.11677601519213</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="B36">
-        <v>0.599362936916089</v>
+        <v>0.13874293945663499</v>
       </c>
       <c r="C36">
-        <v>0.92834609269282897</v>
+        <v>0.11296739067042599</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="B37">
-        <v>0.596964868281185</v>
+        <v>0.28783085452245999</v>
       </c>
       <c r="C37">
-        <v>0.17416469003545099</v>
+        <v>0.112222375489344</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>92</v>
+        <v>23</v>
       </c>
       <c r="B38">
-        <v>0.59337304247759803</v>
+        <v>0.21363013971202099</v>
       </c>
       <c r="C38">
-        <v>0.75245492589179297</v>
+        <v>0.110434017587592</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B39">
-        <v>0.58780330025065697</v>
+        <v>0.13082500782120199</v>
       </c>
       <c r="C39">
-        <v>0.93396899609456596</v>
+        <v>0.10790146972975</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B40">
-        <v>0.58696803697710698</v>
+        <v>0.22075490756737401</v>
       </c>
       <c r="C40">
-        <v>0.68720126458175201</v>
+        <v>0.106109350442252</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="B41">
-        <v>0.576867934730242</v>
+        <v>9.3723855175802201E-2</v>
       </c>
       <c r="C41">
-        <v>0.78676015328792104</v>
+        <v>0.106080245241598</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42">
-        <v>78</v>
+        <v>16</v>
       </c>
       <c r="B42">
-        <v>0.55965033314593504</v>
+        <v>0.23649844294685199</v>
       </c>
       <c r="C42">
-        <v>0.78698655955783703</v>
+        <v>0.10563086784127</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B43">
-        <v>0.55949911671065999</v>
+        <v>0.282482225131715</v>
       </c>
       <c r="C43">
-        <v>0.99243671472129302</v>
+        <v>0.101015306117819</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1091,109 +1093,109 @@
         <v>69</v>
       </c>
       <c r="B44">
-        <v>0.55089526203750605</v>
+        <v>9.2012981170249794E-2</v>
       </c>
       <c r="C44">
-        <v>0.69583286195467897</v>
+        <v>9.5457442641977294E-2</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B45">
-        <v>0.54581173532131799</v>
+        <v>0.23959522680150999</v>
       </c>
       <c r="C45">
-        <v>0.57033125633842396</v>
+        <v>9.2293074638984104E-2</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46">
-        <v>60</v>
-      </c>
-      <c r="B46">
-        <v>0.50267877809991102</v>
+        <v>32</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.21903631264672399</v>
       </c>
       <c r="C46">
-        <v>0.52884593508329403</v>
+        <v>9.2219172796952298E-2</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B47">
-        <v>0.48795119906801598</v>
+        <v>0.11961110201151801</v>
       </c>
       <c r="C47">
-        <v>0.81031639436515901</v>
+        <v>9.1213547720313398E-2</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
-        <v>71</v>
+        <v>6</v>
       </c>
       <c r="B48">
-        <v>0.48191526048989802</v>
+        <v>0.13927242679982099</v>
       </c>
       <c r="C48">
-        <v>6.3064960665017794E-2</v>
+        <v>9.0278958732428694E-2</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B49">
-        <v>0.47851964762430699</v>
+        <v>7.5886257235252899E-2</v>
       </c>
       <c r="C49">
-        <v>0.53302450459772599</v>
+        <v>8.8448742302303304E-2</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B50">
-        <v>0.47851964762430699</v>
+        <v>0.24604965445604199</v>
       </c>
       <c r="C50">
-        <v>0.53302450459772599</v>
+        <v>8.7457854044444297E-2</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B51">
-        <v>0.46446538069166099</v>
+        <v>0.170088548271419</v>
       </c>
       <c r="C51">
-        <v>0.42829806740164</v>
+        <v>8.7094340568491802E-2</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="B52">
-        <v>0.430012167353374</v>
+        <v>0.157140530357611</v>
       </c>
       <c r="C52">
-        <v>0.884860324990001</v>
+        <v>8.6550204908726794E-2</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="B53">
-        <v>0.42150366669794498</v>
+        <v>0.20565544655955501</v>
       </c>
       <c r="C53">
-        <v>0.222755918991172</v>
+        <v>8.4486450478672495E-2</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1201,164 +1203,164 @@
         <v>21</v>
       </c>
       <c r="B54">
-        <v>0.42150366669794498</v>
+        <v>0.21926353963531101</v>
       </c>
       <c r="C54">
-        <v>0.222755918991172</v>
+        <v>8.1536521151351904E-2</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="B55">
-        <v>0.42150366669794498</v>
+        <v>0.23870784436499101</v>
       </c>
       <c r="C55">
-        <v>0.222755918991172</v>
+        <v>8.0799658966371202E-2</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B56">
-        <v>0.42150366669794498</v>
+        <v>0.25001394363755602</v>
       </c>
       <c r="C56">
-        <v>0.222755918991172</v>
+        <v>7.9325153991065794E-2</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="B57">
-        <v>0.38879122559795398</v>
+        <v>0.13891825498536101</v>
       </c>
       <c r="C57">
-        <v>0.45355088553567302</v>
+        <v>7.9270706065733304E-2</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B58">
-        <v>0.37644437855021801</v>
+        <v>0.111980058304118</v>
       </c>
       <c r="C58">
-        <v>0.80977490532521801</v>
+        <v>7.8217885907692394E-2</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="B59">
-        <v>0.37441526147772197</v>
+        <v>0.16122030518278299</v>
       </c>
       <c r="C59">
-        <v>1.9728734871265999E-3</v>
+        <v>7.7111213322654706E-2</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B60">
-        <v>0.36909321613217</v>
+        <v>0.19661160302677699</v>
       </c>
       <c r="C60">
-        <v>0.94582865395905302</v>
+        <v>7.3598102452476694E-2</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B61">
-        <v>0.36184962079489902</v>
+        <v>4.4688508831313999E-2</v>
       </c>
       <c r="C61">
-        <v>1.5951822834761899E-2</v>
+        <v>7.3348247318437795E-2</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B62">
-        <v>0.36184962079489902</v>
+        <v>0.14579692215491499</v>
       </c>
       <c r="C62">
-        <v>1.5951822834761899E-2</v>
+        <v>7.3221574193834502E-2</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B63">
-        <v>0.36184962079489902</v>
+        <v>0.246144417067373</v>
       </c>
       <c r="C63">
-        <v>1.5951822834761899E-2</v>
+        <v>7.1228823622345103E-2</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64">
-        <v>4</v>
+        <v>89</v>
       </c>
       <c r="B64">
-        <v>0.35317473883684902</v>
+        <v>0.109932179715215</v>
       </c>
       <c r="C64">
-        <v>0.605677549132281</v>
+        <v>7.0002679245988395E-2</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65">
-        <v>96</v>
-      </c>
-      <c r="B65">
-        <v>0.33725842914849202</v>
+        <v>1</v>
+      </c>
+      <c r="B65" s="1">
+        <v>6.3635438518691995E-2</v>
       </c>
       <c r="C65">
-        <v>0.76944558082588999</v>
+        <v>6.5470615008155805E-2</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B66">
-        <v>0.32966043923215799</v>
+        <v>0.31903176265212502</v>
       </c>
       <c r="C66">
-        <v>0.179670244936292</v>
+        <v>6.4126501207605505E-2</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B67">
-        <v>0.32937756315966799</v>
+        <v>0.11018880953582</v>
       </c>
       <c r="C67">
-        <v>0.12875489542062099</v>
+        <v>6.23520222997676E-2</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68">
-        <v>70</v>
-      </c>
-      <c r="B68" s="1">
-        <v>0.32849934894517502</v>
+        <v>64</v>
+      </c>
+      <c r="B68">
+        <v>0.20419874075674699</v>
       </c>
       <c r="C68">
-        <v>0.417730337267125</v>
+        <v>5.8819386716015901E-2</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1366,368 +1368,368 @@
         <v>65</v>
       </c>
       <c r="B69">
-        <v>0.32695083644963602</v>
+        <v>0.27913511778425099</v>
       </c>
       <c r="C69">
-        <v>0.46898738146291102</v>
+        <v>5.8696001779995399E-2</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="B70">
-        <v>0.32454977147685798</v>
+        <v>0.17543873628293999</v>
       </c>
       <c r="C70">
-        <v>1.9622903041966001E-2</v>
+        <v>5.6348337361906198E-2</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="B71">
-        <v>0.31131117566531502</v>
+        <v>7.8527828425505805E-2</v>
       </c>
       <c r="C71">
-        <v>2.0756162848575E-2</v>
+        <v>5.6142198592242801E-2</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72">
-        <v>25</v>
+        <v>98</v>
       </c>
       <c r="B72">
-        <v>0.305065050262884</v>
+        <v>7.2613470606034194E-2</v>
       </c>
       <c r="C72">
-        <v>0.26464738226225898</v>
+        <v>5.5721963059786099E-2</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B73">
-        <v>0.30104169043092399</v>
+        <v>0.19672879839434501</v>
       </c>
       <c r="C73">
-        <v>0.227658343138399</v>
+        <v>5.56347848336117E-2</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="B74">
-        <v>0.285576193261875</v>
+        <v>0.14302807879653301</v>
       </c>
       <c r="C74">
-        <v>0.249542249261717</v>
+        <v>5.27567550698732E-2</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="B75">
-        <v>0.27311053697450199</v>
+        <v>0.16661715517279299</v>
       </c>
       <c r="C75">
-        <v>0.96098124753941505</v>
+        <v>5.0777236508593303E-2</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B76">
-        <v>0.27216523108002499</v>
+        <v>0.118885056843116</v>
       </c>
       <c r="C76">
-        <v>0.56746021189958196</v>
+        <v>4.6053216742503199E-2</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="B77">
-        <v>0.26922808056090702</v>
+        <v>5.3851945397269702E-2</v>
       </c>
       <c r="C77">
-        <v>0.72908519542272399</v>
+        <v>4.5835209921039503E-2</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B78">
-        <v>0.25985428860168203</v>
+        <v>0.13041317119311299</v>
       </c>
       <c r="C78">
-        <v>0.96044720984480303</v>
+        <v>4.3820981904822302E-2</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="B79">
-        <v>0.234324443370894</v>
+        <v>0.10505798694540899</v>
       </c>
       <c r="C79">
-        <v>0.86389825205075199</v>
+        <v>4.3195818526419301E-2</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B80">
-        <v>0.18686320236439199</v>
+        <v>0.20480456586236701</v>
       </c>
       <c r="C80">
-        <v>0.92313482652757395</v>
+        <v>4.2618357507635103E-2</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="B81">
-        <v>0.17666646878884601</v>
+        <v>0.21973391301630699</v>
       </c>
       <c r="C81">
-        <v>0.18844246436734199</v>
+        <v>3.87177300648954E-2</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B82">
-        <v>0.172211683408036</v>
+        <v>0.39417118427256298</v>
       </c>
       <c r="C82">
-        <v>0.81756740846442499</v>
+        <v>3.4896247555137198E-2</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B83">
-        <v>0.16379535000342599</v>
+        <v>0.209785080468328</v>
       </c>
       <c r="C83">
-        <v>0.43990456107967202</v>
+        <v>3.30327377140191E-2</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="B84">
-        <v>0.15001692792260299</v>
+        <v>0.21504454493115899</v>
       </c>
       <c r="C84">
-        <v>0.55149636499285404</v>
+        <v>3.2301491939025602E-2</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="B85">
-        <v>0.134132935900411</v>
+        <v>0.18674848024459001</v>
       </c>
       <c r="C85">
-        <v>0.977784004744785</v>
+        <v>2.44705508079818E-2</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="B86">
-        <v>0.122572070493049</v>
+        <v>0.15053236544030099</v>
       </c>
       <c r="C86">
-        <v>0.39976280768397998</v>
+        <v>2.1934360726245002E-2</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="B87">
-        <v>0.117020382718869</v>
+        <v>0.192534211775334</v>
       </c>
       <c r="C87">
-        <v>0.40940448452717199</v>
+        <v>1.8530315291248399E-2</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="B88">
-        <v>0.117020382718869</v>
+        <v>0.42740443865116001</v>
       </c>
       <c r="C88">
-        <v>0.40940448452717199</v>
+        <v>1.51813682070894E-2</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B89">
-        <v>0.114918844520482</v>
+        <v>0.16666620597479101</v>
       </c>
       <c r="C89">
-        <v>0.76592030864147598</v>
+        <v>1.0816775223252299E-2</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="B90">
-        <v>9.8624063476444201E-2</v>
+        <v>0.31819031692459698</v>
       </c>
       <c r="C90">
-        <v>0.54585946710943001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="B91">
-        <v>9.1716595007661494E-2</v>
+        <v>0.24563137013129199</v>
       </c>
       <c r="C91">
-        <v>0.84914421244191596</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B92">
-        <v>8.7514057967843506E-2</v>
+        <v>0.199682933976876</v>
       </c>
       <c r="C92">
-        <v>0.67504053390338403</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="B93">
-        <v>8.3168022991189403E-2</v>
+        <v>0.181433592038453</v>
       </c>
       <c r="C93">
-        <v>0.88767906402437802</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="B94">
-        <v>7.0998858178492705E-2</v>
+        <v>0.16295828381045299</v>
       </c>
       <c r="C94">
-        <v>0.55739630908420301</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="B95">
-        <v>5.9800329900558599E-2</v>
+        <v>0.156503533485333</v>
       </c>
       <c r="C95">
-        <v>0.89613977539746104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B96">
-        <v>5.5365282412294201E-2</v>
+        <v>0.155083473045069</v>
       </c>
       <c r="C96">
-        <v>0.10127765123867501</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97">
+        <v>4</v>
+      </c>
+      <c r="B97">
+        <v>0.126361573112276</v>
+      </c>
+      <c r="C97">
         <v>0</v>
-      </c>
-      <c r="B97">
-        <v>4.6296895400565002E-2</v>
-      </c>
-      <c r="C97">
-        <v>1.1404768794402199E-2</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="B98">
-        <v>4.6296895400565002E-2</v>
+        <v>0.12487545294064099</v>
       </c>
       <c r="C98">
-        <v>1.1404768794402199E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="B99">
-        <v>4.4269185249727297E-2</v>
+        <v>0.12088423370856199</v>
       </c>
       <c r="C99">
-        <v>0.764303486389598</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B100">
-        <v>1.8331808375969299E-2</v>
+        <v>6.9108861164397503E-2</v>
       </c>
       <c r="C100">
-        <v>0.45297667443607997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101">
-        <v>73</v>
-      </c>
-      <c r="B101" s="1">
-        <v>2.7403684536631001E-4</v>
+        <v>95</v>
+      </c>
+      <c r="B101">
+        <v>6.5904653907556093E-2</v>
       </c>
       <c r="C101">
-        <v>0.820503462613421</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F101">
     <sortState ref="A2:F101">
-      <sortCondition descending="1" ref="B1:B101"/>
+      <sortCondition descending="1" ref="C1:C101"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>